<commit_message>
Compare FIM to NIPA-FIM w/o addons
Created alternative FIM and NIPA-FIM scripts with no addons and compared them. The total contributions add up to the same value.
</commit_message>
<xml_diff>
--- a/development/features/nipa-consistent-FIM/results/12-2020/data/fim_interactive.xlsx
+++ b/development/features/nipa-consistent-FIM/results/12-2020/data/fim_interactive.xlsx
@@ -422,19 +422,19 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.4610220021991408</v>
+        <v>-0.04873127066753541</v>
       </c>
       <c r="F2">
-        <v>0.06258375046038947</v>
+        <v>-0.4472294074885931</v>
       </c>
       <c r="G2">
-        <v>0.4946888839019331</v>
+        <v>0.337709939526763</v>
       </c>
       <c r="H2">
-        <v>0.6371181255487443</v>
+        <v>0.0325514381029768</v>
       </c>
       <c r="I2">
-        <v>-0.6707850072515366</v>
+        <v>-0.4189926482972752</v>
       </c>
     </row>
     <row r="3">
@@ -455,19 +455,19 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>-1.377544506626395</v>
+        <v>-1.88755655971204</v>
       </c>
       <c r="F3">
-        <v>-0.2374278903484405</v>
+        <v>-0.7456669684567117</v>
       </c>
       <c r="G3">
-        <v>-0.6648250072254314</v>
+        <v>-0.8258091010027616</v>
       </c>
       <c r="H3">
-        <v>0.1590883676069691</v>
+        <v>-0.4469426647914965</v>
       </c>
       <c r="I3">
-        <v>-0.8718078670079326</v>
+        <v>-0.6148047939177816</v>
       </c>
     </row>
     <row r="4">
@@ -488,19 +488,19 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.1687015292307769</v>
+        <v>-0.3090944267481072</v>
       </c>
       <c r="F4">
-        <v>-0.109460664353942</v>
+        <v>-0.6103231932502593</v>
       </c>
       <c r="G4">
-        <v>0.7419382413465793</v>
+        <v>0.5924702440402585</v>
       </c>
       <c r="H4">
-        <v>-0.03911689401130113</v>
+        <v>-0.6324923326193703</v>
       </c>
       <c r="I4">
-        <v>-0.5341198181045013</v>
+        <v>-0.2690723381689954</v>
       </c>
     </row>
     <row r="5">
@@ -521,19 +521,19 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>-0.6629533436036685</v>
+        <v>-1.107555438830284</v>
       </c>
       <c r="F5">
-        <v>-0.352693579700037</v>
+        <v>-0.8382344239894909</v>
       </c>
       <c r="G5">
-        <v>-0.8358291621042218</v>
+        <v>-0.9830528854812299</v>
       </c>
       <c r="H5">
-        <v>0.5299153898310077</v>
+        <v>-0.03187285342508145</v>
       </c>
       <c r="I5">
-        <v>-0.3570395713304545</v>
+        <v>-0.09262969992397291</v>
       </c>
     </row>
     <row r="6">
@@ -554,19 +554,19 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.1886447405349335</v>
+        <v>-0.2185905956505214</v>
       </c>
       <c r="F6">
-        <v>-0.4207878951160888</v>
+        <v>-0.8806992552352373</v>
       </c>
       <c r="G6">
-        <v>-0.004798706463803183</v>
+        <v>-0.1367743216225977</v>
       </c>
       <c r="H6">
-        <v>0.4375539874872086</v>
+        <v>-0.1043377294862644</v>
       </c>
       <c r="I6">
-        <v>-0.2441105404884718</v>
+        <v>0.02252145545834081</v>
       </c>
     </row>
     <row r="7">
@@ -587,19 +587,19 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1.06957655551899</v>
+        <v>0.6910360014545981</v>
       </c>
       <c r="F7">
-        <v>0.1909923704202574</v>
+        <v>-0.2360511149435778</v>
       </c>
       <c r="G7">
-        <v>0.1167020212982178</v>
+        <v>-0.007530983331492991</v>
       </c>
       <c r="H7">
-        <v>0.9814371046878589</v>
+        <v>0.45983475148806</v>
       </c>
       <c r="I7">
-        <v>-0.02856257046708692</v>
+        <v>0.238732233298031</v>
       </c>
     </row>
     <row r="8">
@@ -620,19 +620,19 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1.383446363398864</v>
+        <v>1.027385345497274</v>
       </c>
       <c r="F8">
-        <v>0.4946785789622792</v>
+        <v>0.09806882811776745</v>
       </c>
       <c r="G8">
-        <v>-0.005555307703252244</v>
+        <v>-0.1229354572108429</v>
       </c>
       <c r="H8">
-        <v>1.277767859852481</v>
+        <v>0.7717753481718346</v>
       </c>
       <c r="I8">
-        <v>0.1112338112496352</v>
+        <v>0.378545454536282</v>
       </c>
     </row>
     <row r="9">
@@ -653,19 +653,19 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1.13522375826276</v>
+        <v>0.8010229583305576</v>
       </c>
       <c r="F9">
-        <v>0.9442228544288863</v>
+        <v>0.5752134274079779</v>
       </c>
       <c r="G9">
-        <v>0.3314497821167763</v>
+        <v>0.2210720097878764</v>
       </c>
       <c r="H9">
-        <v>-0.4053306945159103</v>
+        <v>-0.8904372297481854</v>
       </c>
       <c r="I9">
-        <v>1.209104670661894</v>
+        <v>1.470388178290867</v>
       </c>
     </row>
     <row r="10">
@@ -686,19 +686,19 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>2.23783259464081</v>
+        <v>1.920514942731681</v>
       </c>
       <c r="F10">
-        <v>1.456519817955355</v>
+        <v>1.109989812003529</v>
       </c>
       <c r="G10">
-        <v>-0.1344040332508526</v>
+        <v>-0.2421777842890597</v>
       </c>
       <c r="H10">
-        <v>1.355077793805707</v>
+        <v>0.8988425516396157</v>
       </c>
       <c r="I10">
-        <v>1.017158834085955</v>
+        <v>1.263850175381124</v>
       </c>
     </row>
     <row r="11">
@@ -719,19 +719,19 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>2.599030430822111</v>
+        <v>2.285535806575335</v>
       </c>
       <c r="F11">
-        <v>1.838883286781135</v>
+        <v>1.508614763283713</v>
       </c>
       <c r="G11">
-        <v>0.3783184320669671</v>
+        <v>0.2764802016668795</v>
       </c>
       <c r="H11">
-        <v>0.9206418771130547</v>
+        <v>0.4791857815581942</v>
       </c>
       <c r="I11">
-        <v>1.300070121642089</v>
+        <v>1.529869823350261</v>
       </c>
     </row>
     <row r="12">
@@ -752,19 +752,19 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>2.250525120177156</v>
+        <v>1.931644997024508</v>
       </c>
       <c r="F12">
-        <v>2.055652975975709</v>
+        <v>1.734679676165521</v>
       </c>
       <c r="G12">
-        <v>0.5148298247743641</v>
+        <v>0.4148118483943437</v>
       </c>
       <c r="H12">
-        <v>0.07245834106173334</v>
+        <v>-0.3558433896012271</v>
       </c>
       <c r="I12">
-        <v>1.663236954341059</v>
+        <v>1.872676538231391</v>
       </c>
     </row>
     <row r="13">
@@ -785,19 +785,19 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1.774078688410234</v>
+        <v>1.443739216222842</v>
       </c>
       <c r="F13">
-        <v>2.215366708512577</v>
+        <v>1.895358740638592</v>
       </c>
       <c r="G13">
-        <v>0.1871948514362173</v>
+        <v>0.08638317458400725</v>
       </c>
       <c r="H13">
-        <v>0.2215417545996476</v>
+        <v>-0.1955742236307397</v>
       </c>
       <c r="I13">
-        <v>1.36534208237437</v>
+        <v>1.552930265269574</v>
       </c>
     </row>
     <row r="14">
@@ -818,19 +818,19 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>1.530818646247308</v>
+        <v>1.187712274604289</v>
       </c>
       <c r="F14">
-        <v>2.038613221414201</v>
+        <v>1.712158073606744</v>
       </c>
       <c r="G14">
-        <v>0.3438176679836201</v>
+        <v>0.2434691941703655</v>
       </c>
       <c r="H14">
-        <v>0.2552844291665327</v>
+        <v>-0.1552575279350291</v>
       </c>
       <c r="I14">
-        <v>0.9317165490971551</v>
+        <v>1.099500608368953</v>
       </c>
     </row>
     <row r="15">
@@ -851,19 +851,19 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1.073431936057402</v>
+        <v>0.7133263378476485</v>
       </c>
       <c r="F15">
-        <v>1.657213597723024</v>
+        <v>1.319105706424823</v>
       </c>
       <c r="G15">
-        <v>0.4682780350108303</v>
+        <v>0.3649956239585112</v>
       </c>
       <c r="H15">
-        <v>-0.3784882380687687</v>
+        <v>-0.7862663013077751</v>
       </c>
       <c r="I15">
-        <v>0.9836421391153406</v>
+        <v>1.134597015196912</v>
       </c>
     </row>
     <row r="16">
@@ -884,19 +884,19 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1.766638516168937</v>
+        <v>1.385299507138875</v>
       </c>
       <c r="F16">
-        <v>1.536241946720969</v>
+        <v>1.182519333953415</v>
       </c>
       <c r="G16">
-        <v>-0.05414525130185377</v>
+        <v>-0.1607743612131618</v>
       </c>
       <c r="H16">
-        <v>0.8001125511799414</v>
+        <v>0.391468084836228</v>
       </c>
       <c r="I16">
-        <v>1.020671216290849</v>
+        <v>1.154605783515809</v>
       </c>
     </row>
     <row r="17">
@@ -917,19 +917,19 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0.984721968775601</v>
+        <v>0.588480719753433</v>
       </c>
       <c r="F17">
-        <v>1.338902766812311</v>
+        <v>0.9687047098360626</v>
       </c>
       <c r="G17">
-        <v>-0.0599874683905746</v>
+        <v>-0.1660774104289633</v>
       </c>
       <c r="H17">
-        <v>0.2420652624995633</v>
+        <v>-0.1664084210901077</v>
       </c>
       <c r="I17">
-        <v>0.8026441746666124</v>
+        <v>0.920966551272504</v>
       </c>
     </row>
     <row r="18">
@@ -950,19 +950,19 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1.056035107348324</v>
+        <v>0.6483471362496426</v>
       </c>
       <c r="F18">
-        <v>1.220206882087564</v>
+        <v>0.833863425247401</v>
       </c>
       <c r="G18">
-        <v>0.5174208495565489</v>
+        <v>0.4119572789015341</v>
       </c>
       <c r="H18">
-        <v>-0.04216530301556628</v>
+        <v>-0.4496812402601617</v>
       </c>
       <c r="I18">
-        <v>0.5807795608073409</v>
+        <v>0.6860710976082701</v>
       </c>
     </row>
     <row r="19">
@@ -983,19 +983,19 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0.4993896129206025</v>
+        <v>0.0770642110738915</v>
       </c>
       <c r="F19">
-        <v>1.076696301303365</v>
+        <v>0.6747978935539617</v>
       </c>
       <c r="G19">
-        <v>0.6358926447898382</v>
+        <v>0.5265814199699043</v>
       </c>
       <c r="H19">
-        <v>-0.2879900418715545</v>
+        <v>-0.6971320107002501</v>
       </c>
       <c r="I19">
-        <v>0.1514870100023188</v>
+        <v>0.2476148018042373</v>
       </c>
     </row>
     <row r="20">
@@ -1016,19 +1016,19 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.3149712330409322</v>
+        <v>-0.1197440912471897</v>
       </c>
       <c r="F20">
-        <v>0.7137794805213634</v>
+        <v>0.2985369939574455</v>
       </c>
       <c r="G20">
-        <v>0.3082253456677642</v>
+        <v>0.1939937954892483</v>
       </c>
       <c r="H20">
-        <v>-0.09817299882337999</v>
+        <v>-0.5110391928874694</v>
       </c>
       <c r="I20">
-        <v>0.104918886196548</v>
+        <v>0.1973013061510313</v>
       </c>
     </row>
     <row r="21">
@@ -1049,19 +1049,19 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>-0.0191637718387459</v>
+        <v>-0.4654912699649523</v>
       </c>
       <c r="F21">
-        <v>0.4628080453677766</v>
+        <v>0.03504399652784917</v>
       </c>
       <c r="G21">
-        <v>0.4579664561789401</v>
+        <v>0.3410371559950857</v>
       </c>
       <c r="H21">
-        <v>-0.3143444540806857</v>
+        <v>-0.7326017368471034</v>
       </c>
       <c r="I21">
-        <v>-0.1627857739370003</v>
+        <v>-0.07392668911293453</v>
       </c>
     </row>
     <row r="22">
@@ -1082,19 +1082,19 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>-0.2152046269380691</v>
+        <v>-0.6667320013633875</v>
       </c>
       <c r="F22">
-        <v>0.1449981117961785</v>
+        <v>-0.2937257878754084</v>
       </c>
       <c r="G22">
-        <v>-0.04764254032958169</v>
+        <v>-0.1674425769180218</v>
       </c>
       <c r="H22">
-        <v>0.001415114232938797</v>
+        <v>-0.4183333023237494</v>
       </c>
       <c r="I22">
-        <v>-0.1689772008414262</v>
+        <v>-0.08095612212161635</v>
       </c>
     </row>
     <row r="23">
@@ -1115,19 +1115,19 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>-0.2005026040510668</v>
+        <v>-0.6360786025057473</v>
       </c>
       <c r="F23">
-        <v>-0.02997494244673882</v>
+        <v>-0.4720114912703181</v>
       </c>
       <c r="G23">
-        <v>0.2259279932006186</v>
+        <v>0.1111093650562286</v>
       </c>
       <c r="H23">
-        <v>0.1608372538410204</v>
+        <v>-0.2475996230156754</v>
       </c>
       <c r="I23">
-        <v>-0.5872678510927057</v>
+        <v>-0.4995883445463006</v>
       </c>
     </row>
     <row r="24">
@@ -1148,19 +1148,19 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>-0.647423497727128</v>
+        <v>-1.059035740127721</v>
       </c>
       <c r="F24">
-        <v>-0.2705736251387539</v>
+        <v>-0.7068344034904509</v>
       </c>
       <c r="G24">
-        <v>-0.01692944836407308</v>
+        <v>-0.1286176934788302</v>
       </c>
       <c r="H24">
-        <v>-0.02771452247742881</v>
+        <v>-0.4180221808679609</v>
       </c>
       <c r="I24">
-        <v>-0.6027795268856261</v>
+        <v>-0.5123958657809297</v>
       </c>
     </row>
     <row r="25">
@@ -1181,19 +1181,19 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>-0.3721987206430176</v>
+        <v>-0.7633323808550926</v>
       </c>
       <c r="F25">
-        <v>-0.3588323623398218</v>
+        <v>-0.781294681212986</v>
       </c>
       <c r="G25">
-        <v>0.6052185045210049</v>
+        <v>0.4974004549722678</v>
       </c>
       <c r="H25">
-        <v>-0.3502867946894414</v>
+        <v>-0.7294913180800229</v>
       </c>
       <c r="I25">
-        <v>-0.6271304304745811</v>
+        <v>-0.5312415177473375</v>
       </c>
     </row>
     <row r="26">
@@ -1214,19 +1214,19 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>-0.5013038784080902</v>
+        <v>-0.8684966986355478</v>
       </c>
       <c r="F26">
-        <v>-0.4303571752073271</v>
+        <v>-0.8317358555310261</v>
       </c>
       <c r="G26">
-        <v>0.0710785709364128</v>
+        <v>-0.0354311851550875</v>
       </c>
       <c r="H26">
-        <v>-0.008790751509518233</v>
+        <v>-0.3716284230365846</v>
       </c>
       <c r="I26">
-        <v>-0.5635916978349848</v>
+        <v>-0.4614370904438757</v>
       </c>
     </row>
     <row r="27">
@@ -1247,19 +1247,19 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0.2555307335141176</v>
+        <v>-0.08904151706259722</v>
       </c>
       <c r="F27">
-        <v>-0.316348840816031</v>
+        <v>-0.6949765841702386</v>
       </c>
       <c r="G27">
-        <v>0.864000865716967</v>
+        <v>0.7624212849964971</v>
       </c>
       <c r="H27">
-        <v>0.1069422092253407</v>
+        <v>-0.2430005398580263</v>
       </c>
       <c r="I27">
-        <v>-0.7154123414281901</v>
+        <v>-0.6084622622010679</v>
       </c>
     </row>
     <row r="28">
@@ -1280,19 +1280,19 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>-0.7958771544192893</v>
+        <v>-1.121428329653</v>
       </c>
       <c r="F28">
-        <v>-0.3534622549890713</v>
+        <v>-0.7105747315515585</v>
       </c>
       <c r="G28">
-        <v>-0.06876734097878898</v>
+        <v>-0.1705018602960304</v>
       </c>
       <c r="H28">
-        <v>0.04683716166181404</v>
+        <v>-0.2867973955246156</v>
       </c>
       <c r="I28">
-        <v>-0.7739469751023144</v>
+        <v>-0.6641290738323541</v>
       </c>
     </row>
     <row r="29">
@@ -1313,19 +1313,19 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>-0.5038139482161275</v>
+        <v>-0.8023196183270449</v>
       </c>
       <c r="F29">
-        <v>-0.3863660618823488</v>
+        <v>-0.7203215409195466</v>
       </c>
       <c r="G29">
-        <v>-0.3078566212245543</v>
+        <v>-0.4025810502845579</v>
       </c>
       <c r="H29">
-        <v>0.1955365206213519</v>
+        <v>-0.1206565046774728</v>
       </c>
       <c r="I29">
-        <v>-0.391493847612925</v>
+        <v>-0.2790820633650142</v>
       </c>
     </row>
     <row r="30">
@@ -1346,19 +1346,19 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0.2264405252050647</v>
+        <v>-0.04565329217308323</v>
       </c>
       <c r="F30">
-        <v>-0.20442996097906</v>
+        <v>-0.5146106893039304</v>
       </c>
       <c r="G30">
-        <v>0.9226561346382511</v>
+        <v>0.8359205068024886</v>
       </c>
       <c r="H30">
-        <v>-0.2958138659857579</v>
+        <v>-0.5926581259924339</v>
       </c>
       <c r="I30">
-        <v>-0.4004017434474285</v>
+        <v>-0.2889156729831379</v>
       </c>
     </row>
     <row r="31">
@@ -1379,19 +1379,19 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>-0.3351272645073122</v>
+        <v>-0.5940432398129937</v>
       </c>
       <c r="F31">
-        <v>-0.3520944604844175</v>
+        <v>-0.6408611199915295</v>
       </c>
       <c r="G31">
-        <v>-0.6207245674312992</v>
+        <v>-0.7073973674590198</v>
       </c>
       <c r="H31">
-        <v>0.732959001454615</v>
+        <v>0.4506008967421731</v>
       </c>
       <c r="I31">
-        <v>-0.447361698530628</v>
+        <v>-0.3372467690961469</v>
       </c>
     </row>
     <row r="32">
@@ -1412,19 +1412,19 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0.3097463777574822</v>
+        <v>0.04940884206564128</v>
       </c>
       <c r="F32">
-        <v>-0.07568857744022461</v>
+        <v>-0.3481518270618691</v>
       </c>
       <c r="G32">
-        <v>0.418573520434026</v>
+        <v>0.3357858749249755</v>
       </c>
       <c r="H32">
-        <v>0.2797885772831269</v>
+        <v>-0.007764077025722346</v>
       </c>
       <c r="I32">
-        <v>-0.3886157199596706</v>
+        <v>-0.2786129558336118</v>
       </c>
     </row>
     <row r="33">
@@ -1445,19 +1445,19 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0.1948939905331209</v>
+        <v>-0.06787364306475172</v>
       </c>
       <c r="F33">
-        <v>0.09898840724708748</v>
+        <v>-0.1645403332462959</v>
       </c>
       <c r="G33">
-        <v>0.3870676995564565</v>
+        <v>0.3030696969149382</v>
       </c>
       <c r="H33">
-        <v>-0.03570683215632572</v>
+        <v>-0.3231493194878068</v>
       </c>
       <c r="I33">
-        <v>-0.1564668768670099</v>
+        <v>-0.04779402049188312</v>
       </c>
     </row>
     <row r="34">
@@ -1478,19 +1478,19 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0.5551843985028009</v>
+        <v>0.2930068653878949</v>
       </c>
       <c r="F34">
-        <v>0.1811743755715215</v>
+        <v>-0.07987529385605131</v>
       </c>
       <c r="G34">
-        <v>0.7074003985694142</v>
+        <v>0.6236358189557167</v>
       </c>
       <c r="H34">
-        <v>-0.09925456184085245</v>
+        <v>-0.3814385836201902</v>
       </c>
       <c r="I34">
-        <v>-0.05296143822576081</v>
+        <v>0.05080963005236844</v>
       </c>
     </row>
     <row r="35">
@@ -1511,19 +1511,19 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>0.2092237535793049</v>
+        <v>-0.05500495643225894</v>
       </c>
       <c r="F35">
-        <v>0.3172621300931758</v>
+        <v>0.05488427698913237</v>
       </c>
       <c r="G35">
-        <v>0.3997191853271509</v>
+        <v>0.3150841855461573</v>
       </c>
       <c r="H35">
-        <v>-0.2220240185508833</v>
+        <v>-0.4987027959034622</v>
       </c>
       <c r="I35">
-        <v>0.03152858680303729</v>
+        <v>0.1286136539250459</v>
       </c>
     </row>
     <row r="36">
@@ -1544,19 +1544,19 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>2.862186393722101</v>
+        <v>2.604355249890734</v>
       </c>
       <c r="F36">
-        <v>0.9553721340843303</v>
+        <v>0.6936208789454055</v>
       </c>
       <c r="G36">
-        <v>0.5995147324770616</v>
+        <v>0.5166529743842377</v>
       </c>
       <c r="H36">
-        <v>0.08448158673897618</v>
+        <v>-0.1830553005197068</v>
       </c>
       <c r="I36">
-        <v>2.178190074506063</v>
+        <v>2.270757576026203</v>
       </c>
     </row>
     <row r="37">
@@ -1577,19 +1577,19 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>1.664838263672423</v>
+        <v>1.413474371904714</v>
       </c>
       <c r="F37">
-        <v>1.322858202369156</v>
+        <v>1.063957882687772</v>
       </c>
       <c r="G37">
-        <v>0.6723462386505684</v>
+        <v>0.5925992969432132</v>
       </c>
       <c r="H37">
-        <v>-0.03445495981190488</v>
+        <v>-0.2860140211230767</v>
       </c>
       <c r="I37">
-        <v>1.02694698483376</v>
+        <v>1.106889096084577</v>
       </c>
     </row>
     <row r="38">
@@ -1610,19 +1610,19 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>1.869298898851755</v>
+        <v>1.632737114848932</v>
       </c>
       <c r="F38">
-        <v>1.651386827456395</v>
+        <v>1.398890445053031</v>
       </c>
       <c r="G38">
-        <v>-0.06298272824822171</v>
+        <v>-0.1394235971469711</v>
       </c>
       <c r="H38">
-        <v>0.592144784436984</v>
+        <v>0.3571153873473796</v>
       </c>
       <c r="I38">
-        <v>1.340136842662993</v>
+        <v>1.415045324648523</v>
       </c>
     </row>
     <row r="39">
@@ -1643,19 +1643,19 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>3.745815560885914</v>
+        <v>3.532145216423658</v>
       </c>
       <c r="F39">
-        <v>2.535534779283047</v>
+        <v>2.29567798826701</v>
       </c>
       <c r="G39">
-        <v>-0.9401670276868019</v>
+        <v>-1.010304394238504</v>
       </c>
       <c r="H39">
-        <v>1.84289552569623</v>
+        <v>1.627220873564416</v>
       </c>
       <c r="I39">
-        <v>2.843087062876486</v>
+        <v>2.915228737097745</v>
       </c>
     </row>
     <row r="40">
@@ -1676,19 +1676,19 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>3.066396567514973</v>
+        <v>2.863950898911577</v>
       </c>
       <c r="F40">
-        <v>2.586587322731265</v>
+        <v>2.360576900522221</v>
       </c>
       <c r="G40">
-        <v>-0.6923124432083195</v>
+        <v>-0.7543117229878844</v>
       </c>
       <c r="H40">
-        <v>1.895108765228772</v>
+        <v>1.691007600770912</v>
       </c>
       <c r="I40">
-        <v>1.86360024549452</v>
+        <v>1.927255021128549</v>
       </c>
     </row>
     <row r="41">
@@ -1709,19 +1709,19 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>2.932251685731591</v>
+        <v>2.739523506820382</v>
       </c>
       <c r="F41">
-        <v>2.903440678246056</v>
+        <v>2.692089184251138</v>
       </c>
       <c r="G41">
-        <v>0.4314364861980995</v>
+        <v>0.3756400630062369</v>
       </c>
       <c r="H41">
-        <v>-0.203341095319014</v>
+        <v>-0.4002634009716644</v>
       </c>
       <c r="I41">
-        <v>2.704156294852505</v>
+        <v>2.76414684478581</v>
       </c>
     </row>
     <row r="42">
@@ -1742,19 +1742,19 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>2.449851024240322</v>
+        <v>2.255680791332724</v>
       </c>
       <c r="F42">
-        <v>3.048578709593198</v>
+        <v>2.847825103372086</v>
       </c>
       <c r="G42">
-        <v>0.4126589437105712</v>
+        <v>0.3576683738579091</v>
       </c>
       <c r="H42">
-        <v>-0.2529313794777771</v>
+        <v>-0.4430667021908947</v>
       </c>
       <c r="I42">
-        <v>2.290123460007528</v>
+        <v>2.341079119665709</v>
       </c>
     </row>
     <row r="43">
@@ -1775,19 +1775,19 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1.699251709380812</v>
+        <v>1.494787064688243</v>
       </c>
       <c r="F43">
-        <v>2.536937746716923</v>
+        <v>2.338485565438232</v>
       </c>
       <c r="G43">
-        <v>-0.003475118545377909</v>
+        <v>-0.05919375500843627</v>
       </c>
       <c r="H43">
-        <v>-0.3262867692559824</v>
+        <v>-0.5142971523108247</v>
       </c>
       <c r="I43">
-        <v>2.029013597182172</v>
+        <v>2.068277972007504</v>
       </c>
     </row>
     <row r="44">
@@ -1808,19 +1808,19 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>1.421331716736323</v>
+        <v>1.197042502772429</v>
       </c>
       <c r="F44">
-        <v>2.12567153402226</v>
+        <v>1.921758466403445</v>
       </c>
       <c r="G44">
-        <v>0.4217013248878961</v>
+        <v>0.3644241823176939</v>
       </c>
       <c r="H44">
-        <v>-0.1268230767511501</v>
+        <v>-0.3205134119826434</v>
       </c>
       <c r="I44">
-        <v>1.126453468599577</v>
+        <v>1.153131732437379</v>
       </c>
     </row>
     <row r="45">
@@ -1841,19 +1841,19 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0.4380302649116742</v>
+        <v>0.1913936891530982</v>
       </c>
       <c r="F45">
-        <v>1.502116178817281</v>
+        <v>1.284726011986624</v>
       </c>
       <c r="G45">
-        <v>-0.7703781740154796</v>
+        <v>-0.8313036391249781</v>
       </c>
       <c r="H45">
-        <v>0.1901146834763395</v>
+        <v>-0.01083749490843422</v>
       </c>
       <c r="I45">
-        <v>1.018293755450814</v>
+        <v>1.03353482318651</v>
       </c>
     </row>
     <row r="46">
@@ -1874,19 +1874,19 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>0.4917205565938265</v>
+        <v>0.2280491170529786</v>
       </c>
       <c r="F46">
-        <v>1.012583561905657</v>
+        <v>0.7778180934166878</v>
       </c>
       <c r="G46">
-        <v>0.1696321872222053</v>
+        <v>0.1093803265933912</v>
       </c>
       <c r="H46">
-        <v>-0.696185701270406</v>
+        <v>-0.9040400558173874</v>
       </c>
       <c r="I46">
-        <v>1.018274070642027</v>
+        <v>1.022708846276975</v>
       </c>
     </row>
     <row r="47">
@@ -1907,19 +1907,19 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>-1.153837672331596</v>
+        <v>-1.435554590363258</v>
       </c>
       <c r="F47">
-        <v>0.2993112164775554</v>
+        <v>0.04523267965381267</v>
       </c>
       <c r="G47">
-        <v>0.1684697069789879</v>
+        <v>0.1052663018400833</v>
       </c>
       <c r="H47">
-        <v>-1.191274748505505</v>
+        <v>-1.405178161365769</v>
       </c>
       <c r="I47">
-        <v>-0.1310326308050789</v>
+        <v>-0.1356427308375719</v>
       </c>
     </row>
     <row r="48">
@@ -1940,19 +1940,19 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>-1.023728236607543</v>
+        <v>-1.317036575972885</v>
       </c>
       <c r="F48">
-        <v>-0.3119537718584111</v>
+        <v>-0.5832870900325158</v>
       </c>
       <c r="G48">
-        <v>0.01859064452557019</v>
+        <v>-0.04771455165967983</v>
       </c>
       <c r="H48">
-        <v>-0.5812383154098705</v>
+        <v>-0.8001360962587797</v>
       </c>
       <c r="I48">
-        <v>-0.4610805657232429</v>
+        <v>-0.4691859280544252</v>
       </c>
     </row>
     <row r="49">
@@ -1973,19 +1973,19 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>-1.862090509205113</v>
+        <v>-2.163708922374683</v>
       </c>
       <c r="F49">
-        <v>-0.8869839653876078</v>
+        <v>-1.172062742914461</v>
       </c>
       <c r="G49">
-        <v>0.844913545254637</v>
+        <v>0.7765806304481789</v>
       </c>
       <c r="H49">
-        <v>-2.013634932113948</v>
+        <v>-2.238181795684729</v>
       </c>
       <c r="I49">
-        <v>-0.6933691223458015</v>
+        <v>-0.7021077571381334</v>
       </c>
     </row>
     <row r="50">
@@ -2006,19 +2006,19 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>-0.7825723898975829</v>
+        <v>-1.085197855429415</v>
       </c>
       <c r="F50">
-        <v>-1.20555720201046</v>
+        <v>-1.500374486035059</v>
       </c>
       <c r="G50">
-        <v>0.2562045734879467</v>
+        <v>0.1834550111211309</v>
       </c>
       <c r="H50">
-        <v>-0.3122102720358756</v>
+        <v>-0.5344419343078262</v>
       </c>
       <c r="I50">
-        <v>-0.726566691349654</v>
+        <v>-0.7342109322427203</v>
       </c>
     </row>
     <row r="51">
@@ -2039,19 +2039,19 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>-1.154599503732679</v>
+        <v>-1.457193229872471</v>
       </c>
       <c r="F51">
-        <v>-1.205747659860731</v>
+        <v>-1.505784145912363</v>
       </c>
       <c r="G51">
-        <v>0.1450182149398946</v>
+        <v>0.07071560981847642</v>
       </c>
       <c r="H51">
-        <v>-0.4947906108575231</v>
+        <v>-0.7176627443754469</v>
       </c>
       <c r="I51">
-        <v>-0.804827107815051</v>
+        <v>-0.8102460953155004</v>
       </c>
     </row>
     <row r="52">
@@ -2072,19 +2072,19 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>-0.9787551924122759</v>
+        <v>-1.283561786197311</v>
       </c>
       <c r="F52">
-        <v>-1.194504398811914</v>
+        <v>-1.497415448468469</v>
       </c>
       <c r="G52">
-        <v>-0.4323678523936096</v>
+        <v>-0.5080724268524279</v>
       </c>
       <c r="H52">
-        <v>0.02432447663671006</v>
+        <v>-0.2025417710180311</v>
       </c>
       <c r="I52">
-        <v>-0.5707118166553763</v>
+        <v>-0.572947588326852</v>
       </c>
     </row>
     <row r="53">
@@ -2105,19 +2105,19 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>-0.5541666704975643</v>
+        <v>-0.8579113804721512</v>
       </c>
       <c r="F53">
-        <v>-0.8675234391350274</v>
+        <v>-1.170966062992836</v>
       </c>
       <c r="G53">
-        <v>0.3803818637273209</v>
+        <v>0.3052194895081336</v>
       </c>
       <c r="H53">
-        <v>-0.5017904711965351</v>
+        <v>-0.7312252649849217</v>
       </c>
       <c r="I53">
-        <v>-0.4327580630283501</v>
+        <v>-0.4319056049953631</v>
       </c>
     </row>
     <row r="54">
@@ -2138,19 +2138,19 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>-1.261234603077046</v>
+        <v>-1.566081316743031</v>
       </c>
       <c r="F54">
-        <v>-0.9871889924298931</v>
+        <v>-1.29118692832124</v>
       </c>
       <c r="G54">
-        <v>-0.6673024455224547</v>
+        <v>-0.7446092858195115</v>
       </c>
       <c r="H54">
-        <v>-0.09428784992988173</v>
+        <v>-0.3252187427316049</v>
       </c>
       <c r="I54">
-        <v>-0.4996443076247095</v>
+        <v>-0.4962532881919152</v>
       </c>
     </row>
     <row r="55">
@@ -2171,19 +2171,19 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>-1.479642238239302</v>
+        <v>-1.78341740560202</v>
       </c>
       <c r="F55">
-        <v>-1.068449676056549</v>
+        <v>-1.372742972253628</v>
       </c>
       <c r="G55">
-        <v>-0.4174472957211435</v>
+        <v>-0.4921686592235954</v>
       </c>
       <c r="H55">
-        <v>-0.2709188102602541</v>
+        <v>-0.5060852635372585</v>
       </c>
       <c r="I55">
-        <v>-0.7912761322579049</v>
+        <v>-0.785163482841166</v>
       </c>
     </row>
     <row r="56">
@@ -2204,19 +2204,19 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>-0.9956135774648263</v>
+        <v>-1.29582602246572</v>
       </c>
       <c r="F56">
-        <v>-1.072664272319686</v>
+        <v>-1.37580903132073</v>
       </c>
       <c r="G56">
-        <v>-0.5559174319186626</v>
+        <v>-0.6287230574743243</v>
       </c>
       <c r="H56">
-        <v>0.4227614915339761</v>
+        <v>0.1849357720145109</v>
       </c>
       <c r="I56">
-        <v>-0.8624576370801398</v>
+        <v>-0.8520387370059069</v>
       </c>
     </row>
     <row r="57">
@@ -2237,19 +2237,19 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>-0.8558800173683652</v>
+        <v>-1.152891776480926</v>
       </c>
       <c r="F57">
-        <v>-1.148092609037387</v>
+        <v>-1.449554130322924</v>
       </c>
       <c r="G57">
-        <v>-0.2997224000918609</v>
+        <v>-0.3703343524026967</v>
       </c>
       <c r="H57">
-        <v>-0.1045155710692038</v>
+        <v>-0.3457679880864566</v>
       </c>
       <c r="I57">
-        <v>-0.4516420462073006</v>
+        <v>-0.4367894359917724</v>
       </c>
     </row>
     <row r="58">
@@ -2270,19 +2270,19 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>-1.089777425851169</v>
+        <v>-1.384154271490635</v>
       </c>
       <c r="F58">
-        <v>-1.105228314730917</v>
+        <v>-1.404072369009824</v>
       </c>
       <c r="G58">
-        <v>-0.2240111183472178</v>
+        <v>-0.2932689428279618</v>
       </c>
       <c r="H58">
-        <v>-0.3661740621074557</v>
+        <v>-0.6086125493060102</v>
       </c>
       <c r="I58">
-        <v>-0.4995922453964952</v>
+        <v>-0.4822727793566633</v>
       </c>
     </row>
     <row r="59">
@@ -2303,19 +2303,19 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>-1.005979855269379</v>
+        <v>-1.297127733297141</v>
       </c>
       <c r="F59">
-        <v>-0.9868127189884364</v>
+        <v>-1.282499950933605</v>
       </c>
       <c r="G59">
-        <v>-0.4061811825802247</v>
+        <v>-0.4758609317219583</v>
       </c>
       <c r="H59">
-        <v>0.0958164009158845</v>
+        <v>-0.1457904065771868</v>
       </c>
       <c r="I59">
-        <v>-0.6956150736050389</v>
+        <v>-0.6754763949979962</v>
       </c>
     </row>
     <row r="60">
@@ -2336,19 +2336,19 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>-0.4609466829770461</v>
+        <v>-0.7502484479585232</v>
       </c>
       <c r="F60">
-        <v>-0.8531459953664914</v>
+        <v>-1.146105557306806</v>
       </c>
       <c r="G60">
-        <v>-0.7509726066732845</v>
+        <v>-0.8186692113648987</v>
       </c>
       <c r="H60">
-        <v>0.8413517740071288</v>
+        <v>0.5957517148257038</v>
       </c>
       <c r="I60">
-        <v>-0.5513258503108904</v>
+        <v>-0.5273309514193283</v>
       </c>
     </row>
     <row r="61">
@@ -2369,19 +2369,19 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>0.1144889657936343</v>
+        <v>-0.1723529222894629</v>
       </c>
       <c r="F61">
-        <v>-0.6105537495759914</v>
+        <v>-0.9009708437589398</v>
       </c>
       <c r="G61">
-        <v>-0.0812099604090557</v>
+        <v>-0.145679135076869</v>
       </c>
       <c r="H61">
-        <v>0.5670893333084116</v>
+        <v>0.3184937748295076</v>
       </c>
       <c r="I61">
-        <v>-0.3713904071057216</v>
+        <v>-0.3451675620421015</v>
       </c>
     </row>
     <row r="62">
@@ -2402,19 +2402,19 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>-0.2560740026460129</v>
+        <v>-0.5414991552362339</v>
       </c>
       <c r="F62">
-        <v>-0.4021278937747025</v>
+        <v>-0.6903070646953395</v>
       </c>
       <c r="G62">
-        <v>-0.1957491219772411</v>
+        <v>-0.2593789762831167</v>
       </c>
       <c r="H62">
-        <v>0.1610420819330972</v>
+        <v>-0.08853033153108195</v>
       </c>
       <c r="I62">
-        <v>-0.221366962601869</v>
+        <v>-0.1935898474220352</v>
       </c>
     </row>
     <row r="63">
@@ -2435,19 +2435,19 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>0.3557993770463294</v>
+        <v>0.07521201813555262</v>
       </c>
       <c r="F63">
-        <v>-0.06168308569577541</v>
+        <v>-0.347222126837166</v>
       </c>
       <c r="G63">
-        <v>-0.4074660776168579</v>
+        <v>-0.4697092063682171</v>
       </c>
       <c r="H63">
-        <v>0.7737859440606548</v>
+        <v>0.5264808541056698</v>
       </c>
       <c r="I63">
-        <v>-0.01052048939746758</v>
+        <v>0.01844037039809993</v>
       </c>
     </row>
     <row r="64">
@@ -2468,19 +2468,19 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>0.5639903472426822</v>
+        <v>0.2866904153756362</v>
       </c>
       <c r="F64">
-        <v>0.1945511718591567</v>
+        <v>-0.08798741100362617</v>
       </c>
       <c r="G64">
-        <v>0.06277798709953475</v>
+        <v>0.00252362715707305</v>
       </c>
       <c r="H64">
-        <v>0.5420811257918118</v>
+        <v>0.2957485899681959</v>
       </c>
       <c r="I64">
-        <v>-0.04086876564866442</v>
+        <v>-0.01158180174963275</v>
       </c>
     </row>
     <row r="65">
@@ -2501,19 +2501,19 @@
         <v>0</v>
       </c>
       <c r="E65">
-        <v>0.307228145956788</v>
+        <v>0.03462809556592961</v>
       </c>
       <c r="F65">
-        <v>0.2427359668999451</v>
+        <v>-0.03624215653977805</v>
       </c>
       <c r="G65">
-        <v>-0.1327573957763631</v>
+        <v>-0.1916737660827708</v>
       </c>
       <c r="H65">
-        <v>0.4514429786931769</v>
+        <v>0.20717784504545</v>
       </c>
       <c r="I65">
-        <v>-0.01145743696002578</v>
+        <v>0.01912401660325034</v>
       </c>
     </row>
     <row r="66">
@@ -2534,19 +2534,19 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>0.1650595190470954</v>
+        <v>-0.101181164318189</v>
       </c>
       <c r="F66">
-        <v>0.3480193473232222</v>
+        <v>0.07383734118973317</v>
       </c>
       <c r="G66">
-        <v>-0.1801940834457704</v>
+        <v>-0.237408238522889</v>
       </c>
       <c r="H66">
-        <v>0.4351408046902969</v>
+        <v>0.1939880631619681</v>
       </c>
       <c r="I66">
-        <v>-0.08988720219743118</v>
+        <v>-0.05776098895726807</v>
       </c>
     </row>
     <row r="67">
@@ -2567,19 +2567,19 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>0.5811678301936082</v>
+        <v>0.3179058919803286</v>
       </c>
       <c r="F67">
-        <v>0.4043614606100419</v>
+        <v>0.1345108096509272</v>
       </c>
       <c r="G67">
-        <v>0.1446360764488608</v>
+        <v>0.0884167089163581</v>
       </c>
       <c r="H67">
-        <v>0.5046954554173962</v>
+        <v>0.263932749000691</v>
       </c>
       <c r="I67">
-        <v>-0.06816370167264883</v>
+        <v>-0.0344435659367205</v>
       </c>
     </row>
     <row r="68">
@@ -2600,19 +2600,19 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>-0.2216320364636558</v>
+        <v>-0.4745098658630846</v>
       </c>
       <c r="F68">
-        <v>0.2079558646834573</v>
+        <v>-0.05578926065875303</v>
       </c>
       <c r="G68">
-        <v>-0.3900965921543058</v>
+        <v>-0.4450544600869576</v>
       </c>
       <c r="H68">
-        <v>0.2771373206810341</v>
+        <v>0.04416737387214878</v>
       </c>
       <c r="I68">
-        <v>-0.1086727649903841</v>
+        <v>-0.07362277964827572</v>
       </c>
     </row>
     <row r="69">
@@ -2633,19 +2633,19 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <v>0.1551553537537145</v>
+        <v>-0.09254941770088529</v>
       </c>
       <c r="F69">
-        <v>0.1699376666326889</v>
+        <v>-0.08758363897545676</v>
       </c>
       <c r="G69">
-        <v>-0.08733488089964167</v>
+        <v>-0.1398262108948259</v>
       </c>
       <c r="H69">
-        <v>0.4167077288083179</v>
+        <v>0.1858025198829757</v>
       </c>
       <c r="I69">
-        <v>-0.1742174941549618</v>
+        <v>-0.1385257266890352</v>
       </c>
     </row>
     <row r="70">
@@ -2666,19 +2666,19 @@
         <v>0</v>
       </c>
       <c r="E70">
-        <v>0.04477065697316704</v>
+        <v>-0.1993498198189695</v>
       </c>
       <c r="F70">
-        <v>0.1398654511142069</v>
+        <v>-0.1121258028506519</v>
       </c>
       <c r="G70">
-        <v>-0.1278436839455424</v>
+        <v>-0.1792851824516286</v>
       </c>
       <c r="H70">
-        <v>0.3139223053663386</v>
+        <v>0.08477735595623841</v>
       </c>
       <c r="I70">
-        <v>-0.1413079644476291</v>
+        <v>-0.1048419933235793</v>
       </c>
     </row>
     <row r="71">
@@ -2699,19 +2699,19 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>0.03021909904411188</v>
+        <v>-0.2105616900593193</v>
       </c>
       <c r="F71">
-        <v>0.0021282683268328</v>
+        <v>-0.2442426983605638</v>
       </c>
       <c r="G71">
-        <v>0.2677292251719238</v>
+        <v>0.2174619008522116</v>
       </c>
       <c r="H71">
-        <v>-0.263229069689987</v>
+        <v>-0.4907175487130033</v>
       </c>
       <c r="I71">
-        <v>0.0257189435621751</v>
+        <v>0.06269395780147236</v>
       </c>
     </row>
     <row r="72">
@@ -2732,19 +2732,19 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <v>0.3216049908706686</v>
+        <v>0.07546623696689085</v>
       </c>
       <c r="F72">
-        <v>0.1379375251604139</v>
+        <v>-0.10674867265307</v>
       </c>
       <c r="G72">
-        <v>0.52312767676769</v>
+        <v>0.4713448001377887</v>
       </c>
       <c r="H72">
-        <v>-0.2543557166457277</v>
+        <v>-0.4841068420812866</v>
       </c>
       <c r="I72">
-        <v>0.05283303074870634</v>
+        <v>0.0882282789103888</v>
       </c>
     </row>
     <row r="73">
@@ -2765,19 +2765,19 @@
         <v>0</v>
       </c>
       <c r="E73">
-        <v>0.02813732730488038</v>
+        <v>-0.2288536337787813</v>
       </c>
       <c r="F73">
-        <v>0.1061830185482054</v>
+        <v>-0.140824726672544</v>
       </c>
       <c r="G73">
-        <v>-0.2462085424130513</v>
+        <v>-0.3017482222486264</v>
       </c>
       <c r="H73">
-        <v>0.2811655584663052</v>
+        <v>0.0461165940822635</v>
       </c>
       <c r="I73">
-        <v>-0.006819688748373528</v>
+        <v>0.02677799438758162</v>
       </c>
     </row>
     <row r="74">
@@ -2798,19 +2798,19 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>0.3047075709296589</v>
+        <v>0.03946169552298251</v>
       </c>
       <c r="F74">
-        <v>0.1711672470373284</v>
+        <v>-0.081121847837056</v>
       </c>
       <c r="G74">
-        <v>0.2626719596059693</v>
+        <v>0.2073956322153751</v>
       </c>
       <c r="H74">
-        <v>0.2304793770639839</v>
+        <v>-0.01076315396575835</v>
       </c>
       <c r="I74">
-        <v>-0.1884437657402942</v>
+        <v>-0.1571707827266342</v>
       </c>
     </row>
     <row r="75">
@@ -2831,19 +2831,19 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>0.294044874064441</v>
+        <v>0.01842065120159498</v>
       </c>
       <c r="F75">
-        <v>0.2371236907924106</v>
+        <v>-0.02387626252182744</v>
       </c>
       <c r="G75">
-        <v>0.08774199681802211</v>
+        <v>0.0306947164186419</v>
       </c>
       <c r="H75">
-        <v>0.1651340442225374</v>
+        <v>-0.08217652218718199</v>
       </c>
       <c r="I75">
-        <v>0.04116883302388154</v>
+        <v>0.06990245697013507</v>
       </c>
     </row>
     <row r="76">
@@ -2864,19 +2864,19 @@
         <v>0</v>
       </c>
       <c r="E76">
-        <v>0.7133846925426373</v>
+        <v>0.4273326313133003</v>
       </c>
       <c r="F76">
-        <v>0.3350686162104028</v>
+        <v>0.06409033606477493</v>
       </c>
       <c r="G76">
-        <v>0.4297577362167462</v>
+        <v>0.3711025642848282</v>
       </c>
       <c r="H76">
-        <v>0.07225776655800209</v>
+        <v>-0.181330738092726</v>
       </c>
       <c r="I76">
-        <v>0.2113691897678889</v>
+        <v>0.2375608051211981</v>
       </c>
     </row>
     <row r="77">
@@ -2897,19 +2897,19 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>0.4609231235465978</v>
+        <v>0.1652983376755857</v>
       </c>
       <c r="F77">
-        <v>0.4432650652708321</v>
+        <v>0.1626283289283667</v>
       </c>
       <c r="G77">
-        <v>0.2109924963445054</v>
+        <v>0.149736121517427</v>
       </c>
       <c r="H77">
-        <v>0.226214317730833</v>
+        <v>-0.0320475365984423</v>
       </c>
       <c r="I77">
-        <v>0.0237163094712594</v>
+        <v>0.04760975275660094</v>
       </c>
     </row>
     <row r="78">
@@ -2930,19 +2930,19 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>-0.128762464875444</v>
+        <v>-0.4280824757189858</v>
       </c>
       <c r="F78">
-        <v>0.3348975563195564</v>
+        <v>0.04574228611787459</v>
       </c>
       <c r="G78">
-        <v>0.237122930151244</v>
+        <v>0.1749990815077021</v>
       </c>
       <c r="H78">
-        <v>-0.3937263151375531</v>
+        <v>-0.6542590178924728</v>
       </c>
       <c r="I78">
-        <v>0.02784092011086505</v>
+        <v>0.05117746066578486</v>
       </c>
     </row>
     <row r="79">
@@ -2963,19 +2963,19 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>0.5095737222812375</v>
+        <v>0.2114072310427271</v>
       </c>
       <c r="F79">
-        <v>0.3887797683737556</v>
+        <v>0.09398893107815762</v>
       </c>
       <c r="G79">
-        <v>-0.1472996337848166</v>
+        <v>-0.2106043375194083</v>
       </c>
       <c r="H79">
-        <v>0.5780486871037616</v>
+        <v>0.3193946113555037</v>
       </c>
       <c r="I79">
-        <v>0.07882466896229261</v>
+        <v>0.1026169572066317</v>
       </c>
     </row>
     <row r="80">
@@ -2996,19 +2996,19 @@
         <v>0</v>
       </c>
       <c r="E80">
-        <v>0.9103006332462682</v>
+        <v>0.6139640220240616</v>
       </c>
       <c r="F80">
-        <v>0.4380087535496632</v>
+        <v>0.1406467787558479</v>
       </c>
       <c r="G80">
-        <v>0.3571800727378065</v>
+        <v>0.2937140377981479</v>
       </c>
       <c r="H80">
-        <v>0.502883685661647</v>
+        <v>0.2449579536285602</v>
       </c>
       <c r="I80">
-        <v>0.05023687484681475</v>
+        <v>0.07529203059735352</v>
       </c>
     </row>
     <row r="81">
@@ -3029,19 +3029,19 @@
         <v>0</v>
       </c>
       <c r="E81">
-        <v>0.6941989716365662</v>
+        <v>0.4001201119220791</v>
       </c>
       <c r="F81">
-        <v>0.4963277155721553</v>
+        <v>0.1993522223174713</v>
       </c>
       <c r="G81">
-        <v>0.3494500224676224</v>
+        <v>0.2865971339551443</v>
       </c>
       <c r="H81">
-        <v>0.02425579270840394</v>
+        <v>-0.2340443635458391</v>
       </c>
       <c r="I81">
-        <v>0.3204931564605398</v>
+        <v>0.3475673415127739</v>
       </c>
     </row>
     <row r="82">
@@ -3062,19 +3062,19 @@
         <v>0</v>
       </c>
       <c r="E82">
-        <v>0.773328864734891</v>
+        <v>0.4816080942708356</v>
       </c>
       <c r="F82">
-        <v>0.721850547974739</v>
+        <v>0.4267748648149267</v>
       </c>
       <c r="G82">
-        <v>0.212703570123558</v>
+        <v>0.1490979692537087</v>
       </c>
       <c r="H82">
-        <v>0.2037445872558542</v>
+        <v>-0.05208330323458077</v>
       </c>
       <c r="I82">
-        <v>0.3568807073554788</v>
+        <v>0.3845934282517077</v>
       </c>
     </row>
     <row r="83">
@@ -3095,19 +3095,19 @@
         <v>0</v>
       </c>
       <c r="E83">
-        <v>0.3747326295638803</v>
+        <v>0.08506766165855266</v>
       </c>
       <c r="F83">
-        <v>0.6881402747953997</v>
+        <v>0.395189972468883</v>
       </c>
       <c r="G83">
-        <v>-0.067915184401038</v>
+        <v>-0.1315350366358019</v>
       </c>
       <c r="H83">
-        <v>0.2893119225244437</v>
+        <v>0.03552025383975564</v>
       </c>
       <c r="I83">
-        <v>0.1533358914404745</v>
+        <v>0.181082444454599</v>
       </c>
     </row>
     <row r="84">
@@ -3128,19 +3128,19 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <v>14.58856859453003</v>
+        <v>14.28977758476561</v>
       </c>
       <c r="F84">
-        <v>4.107707265116339</v>
+        <v>3.81414336315427</v>
       </c>
       <c r="G84">
-        <v>7.417972338488096</v>
+        <v>7.353773919383688</v>
       </c>
       <c r="H84">
-        <v>-6.977443138698249</v>
+        <v>-7.240327714345264</v>
       </c>
       <c r="I84">
-        <v>14.14803939474018</v>
+        <v>14.17633137972719</v>
       </c>
     </row>
     <row r="85">
@@ -3161,19 +3161,19 @@
         <v>0</v>
       </c>
       <c r="E85">
-        <v>3.771086318816605</v>
+        <v>3.491222037219344</v>
       </c>
       <c r="F85">
-        <v>4.876929101911349</v>
+        <v>4.586918844478586</v>
       </c>
       <c r="G85">
-        <v>-0.6167606508763772</v>
+        <v>-0.6953801659557474</v>
       </c>
       <c r="H85">
-        <v>-0.3627439242583295</v>
+        <v>-0.5459087627222186</v>
       </c>
       <c r="I85">
-        <v>4.750590893951312</v>
+        <v>4.73251096589731</v>
       </c>
     </row>
     <row r="86">
@@ -3191,19 +3191,19 @@
         <v>1</v>
       </c>
       <c r="E86">
-        <v>-1.350639987943666</v>
+        <v>-1.622913215378336</v>
       </c>
       <c r="F86">
-        <v>4.34593688874171</v>
+        <v>4.060788517066293</v>
       </c>
       <c r="G86">
-        <v>-9.631764796863751</v>
+        <v>-9.701482555767328</v>
       </c>
       <c r="H86">
-        <v>9.701235484812498</v>
+        <v>9.534650587837881</v>
       </c>
       <c r="I86">
-        <v>-1.420110675892413</v>
+        <v>-1.456081247448889</v>
       </c>
     </row>
     <row r="87">
@@ -3221,19 +3221,19 @@
         <v>1</v>
       </c>
       <c r="E87">
-        <v>-1.087475961218586</v>
+        <v>-1.36200474255517</v>
       </c>
       <c r="F87">
-        <v>3.980384741046093</v>
+        <v>3.699020416012863</v>
       </c>
       <c r="G87">
-        <v>0.005436385649192657</v>
+        <v>-0.03354040917632649</v>
       </c>
       <c r="H87">
-        <v>-0.03316271408664977</v>
+        <v>-0.2349071549833028</v>
       </c>
       <c r="I87">
-        <v>-1.059749632781129</v>
+        <v>-1.093557178395541</v>
       </c>
     </row>
     <row r="88">
@@ -3251,19 +3251,19 @@
         <v>1</v>
       </c>
       <c r="E88">
-        <v>-3.794606171292853</v>
+        <v>-4.079925953869371</v>
       </c>
       <c r="F88">
-        <v>-0.6154089504096274</v>
+        <v>-0.8934054686458826</v>
       </c>
       <c r="G88">
-        <v>0.2204877548603792</v>
+        <v>0.1793689729155534</v>
       </c>
       <c r="H88">
-        <v>-0.3840221890700868</v>
+        <v>-0.596252269220499</v>
       </c>
       <c r="I88">
-        <v>-3.631071737083146</v>
+        <v>-3.663042657564426</v>
       </c>
     </row>
     <row r="89">
@@ -3281,19 +3281,19 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <v>-3.965118246203995</v>
+        <v>-4.273250456348833</v>
       </c>
       <c r="F89">
-        <v>-2.549460091664778</v>
+        <v>-2.834523592037927</v>
       </c>
       <c r="G89">
-        <v>-0.2529513690625813</v>
+        <v>-0.2975580548609899</v>
       </c>
       <c r="H89">
-        <v>0.246560888868425</v>
+        <v>0.02194191779816651</v>
       </c>
       <c r="I89">
-        <v>-3.958727766009839</v>
+        <v>-3.99763431928601</v>
       </c>
     </row>
     <row r="90">
@@ -3311,19 +3311,19 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>-4.806461857398988</v>
+        <v>-5.137265094102376</v>
       </c>
       <c r="F90">
-        <v>-3.413415559028608</v>
+        <v>-3.713111561718937</v>
       </c>
       <c r="G90">
-        <v>0.3349910161438696</v>
+        <v>0.2887590868001312</v>
       </c>
       <c r="H90">
-        <v>-0.1706639172200677</v>
+        <v>-0.4102204203808395</v>
       </c>
       <c r="I90">
-        <v>-4.97078895632279</v>
+        <v>-5.015803760521668</v>
       </c>
     </row>
     <row r="91">
@@ -3341,19 +3341,19 @@
         <v>1</v>
       </c>
       <c r="E91">
-        <v>-4.502423993269431</v>
+        <v>-4.845417578078806</v>
       </c>
       <c r="F91">
-        <v>-4.267152567041319</v>
+        <v>-4.583964770599845</v>
       </c>
       <c r="G91">
-        <v>0.3538467513223297</v>
+        <v>0.3049840702027481</v>
       </c>
       <c r="H91">
-        <v>-0.1162734417311298</v>
+        <v>-0.3618140742011701</v>
       </c>
       <c r="I91">
-        <v>-4.739997302860631</v>
+        <v>-4.788587574080385</v>
       </c>
     </row>
     <row r="92">
@@ -3371,19 +3371,19 @@
         <v>1</v>
       </c>
       <c r="E92">
-        <v>-5.857344706289785</v>
+        <v>-6.208437891079021</v>
       </c>
       <c r="F92">
-        <v>-4.782837200790552</v>
+        <v>-5.116092754902258</v>
       </c>
       <c r="G92">
-        <v>0.2548800727433578</v>
+        <v>0.2042127682838731</v>
       </c>
       <c r="H92">
-        <v>-0.01438520712919503</v>
+        <v>-0.2615549877815559</v>
       </c>
       <c r="I92">
-        <v>-6.097839571903948</v>
+        <v>-6.151095671581339</v>
       </c>
     </row>
     <row r="93">
@@ -3401,19 +3401,19 @@
         <v>1</v>
       </c>
       <c r="E93">
-        <v>-4.640399642261666</v>
+        <v>-4.985913232832139</v>
       </c>
       <c r="F93">
-        <v>-4.95165754980497</v>
+        <v>-5.294258449023085</v>
       </c>
       <c r="G93">
-        <v>0.2730930911533709</v>
+        <v>0.2212418418513754</v>
       </c>
       <c r="H93">
-        <v>-0.06803971422453961</v>
+        <v>-0.3165309355356006</v>
       </c>
       <c r="I93">
-        <v>-4.845453019190498</v>
+        <v>-4.890624139147914</v>
       </c>
     </row>
   </sheetData>

</xml_diff>